<commit_message>
updated readme and template file
</commit_message>
<xml_diff>
--- a/data/in/template.xlsx
+++ b/data/in/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\personal-finance-for-newbies\data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6A17A7-3C97-4746-8976-66C781D0E257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D81D9AE-B3E0-47E3-AE01-3167ABBA89D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,19 @@
     <sheet name="Transactions History" sheetId="1" r:id="rId1"/>
     <sheet name="Securities Master Table" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Ticker</t>
   </si>
@@ -74,13 +85,145 @@
   </si>
   <si>
     <t>Bonds</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ticker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: symbol to identify a publicly traded security</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Exchange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: name of the market (according to Yahoo Finance)</t>
+    </r>
+  </si>
+  <si>
+    <t>(this line is just an example, you can remove it)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Shares</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: number of purchased/sold shares; please, include a minus sign to indicate selling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: price of a single share</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Fees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: transaction fees, if any</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Transaction Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: date of transaction in DD/MM/YYYY format</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,8 +238,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +266,14 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -229,11 +392,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -284,9 +459,44 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -504,8 +714,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A1:F32" totalsRowShown="0">
-  <autoFilter ref="A1:F32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A1:F34" totalsRowShown="0">
+  <autoFilter ref="A1:F34" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Exchange"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ticker"/>
@@ -829,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -844,7 +1054,7 @@
     <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.69140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.15234375" customWidth="1"/>
-    <col min="8" max="8" width="42.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -868,26 +1078,27 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="19">
         <v>44525</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="18">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="20">
         <v>99.72</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="20">
         <v>0</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>5</v>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -905,6 +1116,9 @@
       <c r="D4" s="6"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
+      <c r="H4" s="28" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
@@ -913,6 +1127,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
@@ -921,6 +1136,10 @@
       <c r="D6" s="6"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
+      <c r="H6" s="23" t="str">
+        <f>HYPERLINK("https://help.yahoo.com/kb/SLN2310.html", "list of exchange suffixes")</f>
+        <v>list of exchange suffixes</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
@@ -929,6 +1148,9 @@
       <c r="D7" s="6"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
+      <c r="H7" s="28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="6"/>
@@ -937,6 +1159,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="6"/>
@@ -945,6 +1168,9 @@
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
+      <c r="H9" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="6"/>
@@ -953,6 +1179,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="6"/>
@@ -961,6 +1188,9 @@
       <c r="D11" s="6"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
+      <c r="H11" s="28" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="6"/>
@@ -969,6 +1199,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="6"/>
@@ -977,6 +1208,9 @@
       <c r="D13" s="6"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
+      <c r="H13" s="24" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="6"/>
@@ -985,6 +1219,9 @@
       <c r="D14" s="6"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
+      <c r="H14" s="24" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="6"/>
@@ -1074,7 +1311,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1082,7 +1319,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -1107,20 +1344,20 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="9"/>
@@ -1130,11 +1367,33 @@
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H9:H10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1175,22 +1434,23 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="27" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>